<commit_message>
Fixed the hyperlink in excel
-Fixed some bugs in js and html
</commit_message>
<xml_diff>
--- a/Excel Test/New Microsoft Excel Worksheet.xlsx
+++ b/Excel Test/New Microsoft Excel Worksheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7196BE62-304D-40F5-944D-0BFC398B402E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95B3AF77-974E-4A5B-B0B4-DBF5ED540236}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18192" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -243,6 +243,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -543,7 +547,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,7 +610,7 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E4" t="s">
@@ -626,7 +630,7 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>48</v>
       </c>
       <c r="E5" t="s">
@@ -850,13 +854,14 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://www.google.com/" xr:uid="{D30916B6-7F3A-46A8-AFA8-3AC389192C47}"/>
+    <hyperlink ref="A4" r:id="rId1" display="https://www.google.com/" xr:uid="{D30916B6-7F3A-46A8-AFA8-3AC389192C47}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{08B7D8FA-54EC-4B4A-8EEF-F1D1D75F1EFB}"/>
+    <hyperlink ref="D5" r:id="rId3" display="https://www.google.com/" xr:uid="{987149B4-D492-4830-89A1-DCD7B5D0CCB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>